<commit_message>
Incorporación de bees al Lector, Valuador y Sesionador
</commit_message>
<xml_diff>
--- a/archivos/serenisima-ACTUALIZADO.xlsx
+++ b/archivos/serenisima-ACTUALIZADO.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>907,38</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>907,38</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>942,72</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -630,7 +630,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>1.248,26</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>1.384,14</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -704,7 +704,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>1.310,41</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>676,99</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -844,7 +844,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>676,99</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>232,90</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>1.671,37</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>1.671,37</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1697,7 +1697,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>552,99</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>815,64</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>815,64</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>393,16</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1911,7 +1911,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>552,99</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>393,16</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">

</xml_diff>

<commit_message>
Comienzo de integración a la GUI
</commit_message>
<xml_diff>
--- a/archivos/serenisima-ACTUALIZADO.xlsx
+++ b/archivos/serenisima-ACTUALIZADO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>907,38</t>
+          <t>952,75</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -531,32 +531,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3570</t>
+          <t>3571</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CREMA DE LECHE LA SERENISIMA P/COCINAR X 200 ML</t>
+          <t>CREMA DE LECHE LA SERENISIMA P/BATIR X 200 ML</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7790742141606</t>
+          <t>7790742011701</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>330100</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>907,38</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -568,32 +564,28 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5749</t>
+          <t>3570</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DULCE DE LECHE LA SERENISIMA 250GRS</t>
+          <t>CREMA DE LECHE LA SERENISIMA P/COCINAR X 200 ML</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7790742104809</t>
+          <t>7790742141606</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>104800</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>942,72</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -605,32 +597,28 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>479</t>
+          <t>3570</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DULCE DE LECHE LA SERENISIMA CLASICO X 400 GR</t>
+          <t>CREMA DE LECHE LA SERENISIMA P/COCINAR X 200 ML</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7790742625304</t>
+          <t>7790742141606</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>625300</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1.248,26</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -642,32 +630,32 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1097</t>
+          <t>5749</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DULCE DE LECHE LA SERENISIMA COLONIAL X 400GRS</t>
+          <t>DULCE DE LECHE LA SERENISIMA 250GRS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7790742625205</t>
+          <t>7790742104809</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>625200</t>
+          <t>104800</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1.384,14</t>
+          <t>989,86</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -679,32 +667,32 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1098</t>
+          <t>5749</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DULCE DE LECHE LA SERENISIMA TRADICION X 400 GR</t>
+          <t>DULCE DE LECHE LA SERENISIMA 250GRS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7790742625502</t>
+          <t>7790742104809</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>625500</t>
+          <t>104800</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1.310,41</t>
+          <t>989,86</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -716,28 +704,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5855</t>
+          <t>479</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LECHE ARMONIA 1% TETRAPACK 1,0LT</t>
+          <t>DULCE DE LECHE LA SERENISIMA CLASICO X 400 GR</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7793940361005</t>
+          <t>7790742625304</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>625300</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>1.310,67</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -749,28 +741,32 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5854</t>
+          <t>479</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LECHE ARMONIA 2% TETRAPACK 1,0LT</t>
+          <t>DULCE DE LECHE LA SERENISIMA CLASICO X 400 GR</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7790742336200</t>
+          <t>7790742625304</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>625300</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>1.310,67</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -782,32 +778,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3355</t>
+          <t>1097</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LECHE ARMONIA DESCR. 1% X1LT</t>
+          <t>DULCE DE LECHE LA SERENISIMA COLONIAL X 400GRS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>7790742430601</t>
+          <t>7790742625205</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>430600</t>
+          <t>625200</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>676,99</t>
+          <t>1.453,35</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -819,32 +815,32 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>1097</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LECHE ARMONIA ENTERA 2% SACHET 1 LITRO</t>
+          <t>DULCE DE LECHE LA SERENISIMA COLONIAL X 400GRS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>7790742430700</t>
+          <t>7790742625205</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>430700</t>
+          <t>625200</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>676,99</t>
+          <t>1.453,35</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -856,28 +852,32 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>5411</t>
+          <t>1098</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LECHE LA SER. DESCREMADA 0%</t>
+          <t>DULCE DE LECHE LA SERENISIMA TRADICION X 400 GR</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7790742034502</t>
+          <t>7790742625502</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>625500</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>1.375,93</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -889,22 +889,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3383</t>
+          <t>5855</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LECHE LA SERENISIMA  TETRA PACK X2% X 1 LT</t>
+          <t>LECHE ARMONIA 1% TETRAPACK 1,0LT</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7790742357403</t>
+          <t>7793940361005</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -922,29 +922,25 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5903</t>
+          <t>5854</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LECHE LA SERENISIMA 1% TETRAPACK 1,0LT</t>
+          <t>LECHE ARMONIA 2% TETRAPACK 1,0LT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>7790742363107</t>
+          <t>7790742336200</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>449100</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
           <t>Sin precio</t>
@@ -959,28 +955,32 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5423</t>
+          <t>3355</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LECHE LA SERENISIMA DESCREMADA MULTIVITAMINAS SACHET 1,0LT</t>
+          <t>LECHE ARMONIA DESCR. 1% X1LT</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>7790742348005</t>
+          <t>7790742430601</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>430600</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>710,84</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -992,32 +992,32 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>424</t>
+          <t>3355</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LECHE LA SERENISIMA DESCREMADA SACHET 1,0LT</t>
+          <t>LECHE ARMONIA DESCR. 1% X1LT</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7790742449108</t>
+          <t>7790742430601</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>449100</t>
+          <t>430600</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>710,84</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1029,22 +1029,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3399</t>
+          <t>5399</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LECHE LA SERENISIMA ENTERA 3% ENV. SUSTENTABLEX1LT</t>
+          <t>LECHE ARMONIA ENTERA 2% SACHET 1 LITRO</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7790742363008</t>
+          <t>7790742430700</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1062,29 +1062,25 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>423</t>
+          <t>5399</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LECHE LA SERENISIMA ENTERA SACHET 1,0LT</t>
+          <t>LECHE ARMONIA ENTERA 2% SACHET 1 LITRO</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7790742448002</t>
+          <t>7790742430700</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>244800</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
           <t>Sin precio</t>
@@ -1099,22 +1095,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>978</t>
+          <t>5411</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LECHE LA SERENISIMA ENTERA TETRAPACK 1,0LT</t>
+          <t>LECHE LA SER. DESCREMADA 0%</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7790742308801</t>
+          <t>7790742034502</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1132,22 +1128,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5379</t>
+          <t>3383</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LECHE LA SERENISIMA SEMI DESCREMADA 2% SACHET 1LT</t>
+          <t>LECHE LA SERENISIMA  TETRA PACK X2% X 1 LT</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>7790742044921</t>
+          <t>7790742357403</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1165,22 +1161,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4994</t>
+          <t>5903</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LECHE SERENISSIMA TETRA DESCREMADA POR 1LT</t>
+          <t>LECHE LA SERENISIMA 1% TETRAPACK 1,0LT</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7790742357106</t>
+          <t>7790742363107</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1198,32 +1194,28 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>5423</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LEVADURA CALSA CUBO FRESCA TETRAPACK 50GRS</t>
+          <t>LECHE LA SERENISIMA DESCREMADA MULTIVITAMINAS SACHET 1,0LT</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7790813110401</t>
+          <t>7790742348005</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>394000</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>232,90</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1235,22 +1227,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>424</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MANTECA LA SERENISIMA CLASICA ORIGINAL PAQUETE 100GRS</t>
+          <t>LECHE LA SERENISIMA DESCREMADA SACHET 1,0LT</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>7793940052002</t>
+          <t>7790742449108</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -1268,22 +1260,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4448</t>
+          <t>424</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MANTECA LA SERENISIMA POR 100 GRS</t>
+          <t>LECHE LA SERENISIMA DESCREMADA SACHET 1,0LT</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7790742034526</t>
+          <t>7790742449108</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1301,22 +1293,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4269</t>
+          <t>3399</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MANTECA LA SERENISIMA POR 200 GRS</t>
+          <t>LECHE LA SERENISIMA ENTERA 3% ENV. SUSTENTABLEX1LT</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7790742345806</t>
+          <t>7790742363008</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1334,25 +1326,29 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5477</t>
+          <t>423</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MANTECA LA SERENISIMA X 200 G</t>
+          <t>LECHE LA SERENISIMA ENTERA SACHET 1,0LT</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>7793940054006</t>
+          <t>7790742448002</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>244800</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>Sin precio</t>
@@ -1367,32 +1363,32 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5252</t>
+          <t>423</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>QUESO CREMA CASANCREM LIGHT X 290 GR</t>
+          <t>LECHE LA SERENISIMA ENTERA SACHET 1,0LT</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>7791337060791</t>
+          <t>7790742448002</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>613800</t>
+          <t>244800</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1.671,37</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1404,22 +1400,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4183</t>
+          <t>978</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>QUESO CREMA LIGHT LA PAULINA POR 290 GRS</t>
+          <t>LECHE LA SERENISIMA ENTERA TETRAPACK 1,0LT</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>7794990879663</t>
+          <t>7790742308801</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>RIDISA S.A. (LA PAULINA),LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1437,32 +1433,28 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5261</t>
+          <t>978</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>QUESO LA SERENISIMA CASANCREM CLASICO 290GRS</t>
+          <t>LECHE LA SERENISIMA ENTERA TETRAPACK 1,0LT</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>7791337060784</t>
+          <t>7790742308801</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>613600</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>1.671,37</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1474,22 +1466,22 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>401</t>
+          <t>5379</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>QUESO LA SERENISIMA CHEDDAR X KG</t>
+          <t>LECHE LA SERENISIMA SEMI DESCREMADA 2% SACHET 1LT</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>710</t>
+          <t>7790742044921</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1507,22 +1499,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1043</t>
+          <t>4994</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>QUESO LA SERENISIMA CREMON SIMPLE X KG</t>
+          <t>LECHE SERENISSIMA TETRA DESCREMADA POR 1LT</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>711</t>
+          <t>7790742357106</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1540,28 +1532,32 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>888</t>
+          <t>320</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>QUESO LA SERENISIMA CREMOSO CREMON LIGHT X KG</t>
+          <t>LEVADURA CALSA CUBO FRESCA TETRAPACK 50GRS</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>740</t>
+          <t>7790813110401</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>394000</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>263,18</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1573,22 +1569,22 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>889</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>QUESO LA SERENISIMA CREMOSO DOBLE CREMA X KG</t>
+          <t>MANTECA LA SERENISIMA CLASICA ORIGINAL PAQUETE 100GRS</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>7793940052002</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -1606,22 +1602,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>QUESO LA SERENISIMA DANBO X KG</t>
+          <t>MANTECA LA SERENISIMA CLASICA ORIGINAL PAQUETE 100GRS</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>713</t>
+          <t>7793940052002</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1639,22 +1635,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>909</t>
+          <t>4448</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>QUESO LA SERENISIMA PATEGRAS X KG</t>
+          <t>MANTECA LA SERENISIMA POR 100 GRS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>827</t>
+          <t>7790742034526</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -1672,32 +1668,28 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5069</t>
+          <t>4269</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>YOGUR SER FIRME VAINILLA POR 190 GR</t>
+          <t>MANTECA LA SERENISIMA POR 200 GRS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>7791337005228</t>
+          <t>7790742345806</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>610401</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>552,99</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1709,22 +1701,22 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5039</t>
+          <t>5477</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>YOGURT LA SER FIRME VAINILLA POR 190 GRS</t>
+          <t>MANTECA LA SERENISIMA X 200 G</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>7791337004757</t>
+          <t>7793940054006</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1742,32 +1734,28 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5066</t>
+          <t>5477</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>YOGURT LA SERENISIMA CON CEREAL POR 159</t>
+          <t>MANTECA LA SERENISIMA X 200 G</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>7791337007390</t>
+          <t>7793940054006</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>610700</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>815,64</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1779,32 +1767,32 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5065</t>
+          <t>5252</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>YOGURT LA SERENISIMA CON ROCKLETS 164G</t>
+          <t>QUESO CREMA CASANCREM LIGHT X 290 GR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>7791337007383</t>
+          <t>7791337060791</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>610600</t>
+          <t>613800</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>815,64</t>
+          <t>1.987,62</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1816,22 +1804,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6930</t>
+          <t>4183</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>YOGURT LA SERENISIMA CREMIX VAINILLA 120GRS</t>
+          <t>QUESO CREMA LIGHT LA PAULINA POR 290 GRS</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>7791337007567</t>
+          <t>7794990879663</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -1849,32 +1837,32 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5691</t>
+          <t>5261</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>YOGURT LA SERENISIMA FIRME FRUTILLA 120GRS</t>
+          <t>QUESO LA SERENISIMA CASANCREM CLASICO 290GRS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>7791337007437</t>
+          <t>7791337060784</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>610502</t>
+          <t>613600</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>393,16</t>
+          <t>1.987,62</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1886,32 +1874,28 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5710</t>
+          <t>401</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>YOGURT LA SERENISIMA FIRME VAINILLA 190GRS</t>
+          <t>QUESO LA SERENISIMA CHEDDAR X KG</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>7791337007444</t>
+          <t>710</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>610402</t>
-        </is>
-      </c>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>552,99</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -1923,22 +1907,22 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5720</t>
+          <t>401</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>YOGURT LA SERENISIMA YOGURISIMO FRUTILLA 120GRS</t>
+          <t>QUESO LA SERENISIMA CHEDDAR X KG</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>7791337007598</t>
+          <t>710</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>LA SERENISIMA S.A</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -1956,22 +1940,22 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5422</t>
+          <t>1043</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>YOGURT SER COLCHON DUR/MAN 175G</t>
+          <t>QUESO LA SERENISIMA CREMON SIMPLE X KG</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>7791337006928</t>
+          <t>711</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>LOGISTICA LA SERENISIMA</t>
+          <t>LA SERENISIMA</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1989,37 +1973,688 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>1043</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>QUESO LA SERENISIMA CREMON SIMPLE X KG</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>711</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>888</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>QUESO LA SERENISIMA CREMOSO CREMON LIGHT X KG</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>740</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>888</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>QUESO LA SERENISIMA CREMOSO CREMON LIGHT X KG</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>740</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>889</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>QUESO LA SERENISIMA CREMOSO DOBLE CREMA X KG</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>765</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>404</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>QUESO LA SERENISIMA DANBO X KG</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>713</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>404</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>QUESO LA SERENISIMA DANBO X KG</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>713</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>909</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>QUESO LA SERENISIMA PATEGRAS X KG</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>827</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>909</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>QUESO LA SERENISIMA PATEGRAS X KG</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>827</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>5069</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>YOGUR SER FIRME VAINILLA POR 190 GR</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>7791337005228</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>610401</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>642,58</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>5039</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>YOGURT LA SER FIRME VAINILLA POR 190 GRS</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>7791337004757</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>5066</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>YOGURT LA SERENISIMA CON CEREAL POR 159</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>7791337007390</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>610700</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>900,97</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>5065</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>YOGURT LA SERENISIMA CON ROCKLETS 164G</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>7791337007383</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>610600</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>900,97</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>6930</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>YOGURT LA SERENISIMA CREMIX VAINILLA 120GRS</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>7791337007567</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2024-02-02 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>5691</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>YOGURT LA SERENISIMA FIRME FRUTILLA 120GRS</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>7791337007437</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>610502</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>426,22</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2024-01-17 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>5710</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>YOGURT LA SERENISIMA FIRME VAINILLA 190GRS</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>7791337007444</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>610402</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>642,58</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2024-01-26 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>5720</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>YOGURT LA SERENISIMA YOGURISIMO FRUTILLA 120GRS</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>7791337007598</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2024-02-19 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>5720</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>YOGURT LA SERENISIMA YOGURISIMO FRUTILLA 120GRS</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>7791337007598</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2024-01-17 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>5422</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>YOGURT SER COLCHON DUR/MAN 175G</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>7791337006928</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
           <t>5448</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B64" t="inlineStr">
         <is>
           <t>YOGURT SER FIRME VAINILLA 120GRS</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C64" t="inlineStr">
         <is>
           <t>7791337007604</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>LA SERENISIMA S.A</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
         <is>
           <t>610501</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>393,16</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>2024-01-26 00:00:00</t>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>426,22</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2024-01-11 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>5448</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>YOGURT SER FIRME VAINILLA 120GRS</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>7791337007604</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>LA SERENISIMA</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>610501</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>426,22</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2024-01-11 00:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>